<commit_message>
DOM Changes in ECTEST2
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC6_SearchResults_Typeahead.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC6_SearchResults_Typeahead.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A48EAE6-E17C-4D2B-B16A-FD1984301015}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCA81DE-3D0A-4CBF-8CBD-7EA528830F16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC6_SearchResults_Typeahead" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>PRESS_ENTER</t>
   </si>
   <si>
-    <t>ValidSearchHeader</t>
-  </si>
-  <si>
     <t>validSearchV</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Showing Results for "sprocket"</t>
+  </si>
+  <si>
+    <t>ValidSearchHeader1</t>
   </si>
 </sst>
 </file>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -551,7 +551,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -565,13 +565,13 @@
     <row r="3" spans="1:5">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -584,7 +584,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>12</v>
@@ -593,7 +593,7 @@
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
@@ -608,7 +608,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>14</v>
@@ -623,23 +623,23 @@
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -676,7 +676,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -697,7 +697,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -705,15 +705,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
@@ -729,21 +729,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -940,24 +925,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -974,4 +957,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>